<commit_message>
update database for lectures
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holynomad/Documents/다이나믹샤크_벤치마크/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holynomad/Documents/다이나믹샤크_벤치마크/다샤봇/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A77E4F-9420-B545-A114-49941DD38B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D09C8D2-63C1-6C44-9C53-3CF5CACD9406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="27780" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="2580" windowWidth="27780" windowHeight="15420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="3" r:id="rId1"/>
-    <sheet name="Content" sheetId="2" r:id="rId2"/>
-    <sheet name="Response" sheetId="4" r:id="rId3"/>
+    <sheet name="Response" sheetId="4" r:id="rId2"/>
+    <sheet name="Lecture" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="test__4" localSheetId="1">Content!$A$1:$L$6</definedName>
+    <definedName name="test__4" localSheetId="2">Lecture!$A$1:$L$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390BC996-DE05-5B43-8485-940A24944A2C}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1388,11 +1388,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6B3B04-2CEE-A84E-8C1C-73E3450B8318}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="133">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1627,89 +1712,4 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6B3B04-2CEE-A84E-8C1C-73E3450B8318}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
-  <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="133">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
don't care it's just exercise for chatbot
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holynomad/Documents/다이나믹샤크_벤치마크/다샤봇/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D09C8D2-63C1-6C44-9C53-3CF5CACD9406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2435414-3953-934E-9E22-7054EC76A6C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="2580" windowWidth="27780" windowHeight="15420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="1620" windowWidth="27780" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="3" r:id="rId1"/>
@@ -58,10 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
-  <si>
-    <t>Link</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
   <si>
     <t>Video Id</t>
   </si>
@@ -290,6 +287,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>이세하</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>중</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -322,10 +323,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>맥가이버</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>산업군</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -347,6 +344,30 @@
   </si>
   <si>
     <t>flask 챗봇만들기</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>해시태그</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>#백엔드 #backend #백엔드개발 #딜리버리히어로</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>#백엔드 #backend #백엔드개발 #로또추천</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>#코딩테스트 #개발 #웹개발</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>#취업준비 #취준 #개발</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>#백엔드 #backend #백엔드개발 #기본원리</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1308,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390BC996-DE05-5B43-8485-940A24944A2C}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1319,25 +1340,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
       <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
-        <v>82</v>
-      </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" t="s">
         <v>71</v>
@@ -1357,19 +1378,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
         <v>83</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
       </c>
       <c r="F2" t="s">
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
         <v>74</v>
@@ -1407,63 +1428,63 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="133">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1476,13 +1497,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
@@ -1497,63 +1518,66 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
       </c>
       <c r="I2">
         <v>46306</v>
@@ -1562,33 +1586,36 @@
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
       </c>
       <c r="I3">
         <v>24873</v>
@@ -1597,33 +1624,36 @@
         <v>203</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
       </c>
       <c r="I4">
         <v>16189</v>
@@ -1632,33 +1662,36 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>41</v>
-      </c>
-      <c r="H5" t="s">
-        <v>42</v>
       </c>
       <c r="I5">
         <v>14279</v>
@@ -1667,33 +1700,36 @@
         <v>115</v>
       </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
       <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>46</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>47</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>49</v>
       </c>
       <c r="I6">
         <v>11679</v>
@@ -1702,7 +1738,7 @@
         <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
         <v>70</v>

</xml_diff>